<commit_message>
edit ergm description table
</commit_message>
<xml_diff>
--- a/analysis/data/raw_data/ergm_term.xlsx
+++ b/analysis/data/raw_data/ergm_term.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/EmilyWang/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/EmilyWang/Desktop/School document/LW-Papers/kwl-burials-2020/analysis/data/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{137C90FD-C5E3-F64F-B68E-F08B009C93D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82BD63F9-7601-834D-99FC-DCD15E87A46C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="43840" yWindow="1200" windowWidth="20020" windowHeight="18660" xr2:uid="{9B72E976-F785-7749-915A-031B6E0C4CD8}"/>
+    <workbookView xWindow="30820" yWindow="2440" windowWidth="20020" windowHeight="16560" xr2:uid="{9B72E976-F785-7749-915A-031B6E0C4CD8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,13 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
-  <si>
-    <t>Configurations (effect)</t>
-  </si>
-  <si>
-    <t>Property</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>Description</t>
   </si>
@@ -53,85 +47,100 @@
     <t>Density</t>
   </si>
   <si>
-    <t>Numer of ties in the network</t>
-  </si>
-  <si>
     <t xml:space="preserve">Tendency for nodes with shared partners to be tied </t>
   </si>
   <si>
-    <t xml:space="preserve">Geometrically weighted non-edgewise shared partner </t>
-  </si>
-  <si>
-    <t>Geometrically weighted edgewise shared partner</t>
-  </si>
-  <si>
-    <t>Multiple connectivity</t>
-  </si>
-  <si>
-    <t>Cohesion or transitivity</t>
-  </si>
-  <si>
-    <t>geometrically weighted degree distribution</t>
-  </si>
-  <si>
     <t>Popularity</t>
   </si>
   <si>
     <t>Tendency towards centralization in distribution</t>
   </si>
   <si>
-    <t>Tendency of nondirectly connected nodes to be connected through multiple others</t>
-  </si>
-  <si>
-    <t>Density of ties between nodes with same gender</t>
-  </si>
-  <si>
-    <t>Density of ties between nodes with same age</t>
-  </si>
-  <si>
     <t>Density of ties between nodes with same scale of wealth</t>
   </si>
   <si>
     <t>Density of ties between nodes with same ritual treatment</t>
   </si>
   <si>
-    <t>Node covariate  (gender)</t>
-  </si>
-  <si>
-    <t>Node covariate  (age)</t>
-  </si>
-  <si>
-    <t>Node covariate  (wealth)</t>
-  </si>
-  <si>
-    <t>Node covariate (ritual)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Homophily </t>
-  </si>
-  <si>
-    <t>burial having the same gender to be connected</t>
-  </si>
-  <si>
-    <t>burial having the same age to be connected</t>
-  </si>
-  <si>
-    <t>burial having the same scale of wealth to be connected</t>
-  </si>
-  <si>
-    <t>burial having the same ritual treatment to be connected</t>
-  </si>
-  <si>
-    <t>burial being connected with mutiple partners</t>
-  </si>
-  <si>
-    <t>two burial having relationship</t>
-  </si>
-  <si>
-    <t xml:space="preserve">burial to be connected with a third shared burial </t>
-  </si>
-  <si>
-    <t xml:space="preserve">burial to be connected without a third shared burial </t>
+    <t>Density of ties between nodes with the same age</t>
+  </si>
+  <si>
+    <t>Density of ties between nodes with the same gender</t>
+  </si>
+  <si>
+    <t>Network Property</t>
+  </si>
+  <si>
+    <t>Configurations (effect/parameter)</t>
+  </si>
+  <si>
+    <t>Transitivity or cohesion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Homophily/nodematch.age </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Homophily/nodematch.sex </t>
+  </si>
+  <si>
+    <t>Node covariate of age</t>
+  </si>
+  <si>
+    <t>Node covariate of sex</t>
+  </si>
+  <si>
+    <t>Node covariate of ritual pottery</t>
+  </si>
+  <si>
+    <t>Node covariate of burial value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Homophily/nodematch.value </t>
+  </si>
+  <si>
+    <t>Homophily/nodematch.ritual</t>
+  </si>
+  <si>
+    <t>Geometrically weighted edgewise shared partner (gwesp)</t>
+  </si>
+  <si>
+    <t>geometrically weighted degree distribution (gwdeg)</t>
+  </si>
+  <si>
+    <t>physical distance</t>
+  </si>
+  <si>
+    <t>Distance (in meter) between each pairs of burials</t>
+  </si>
+  <si>
+    <t>two burials having relationship</t>
+  </si>
+  <si>
+    <t>burials having the same age to be connected</t>
+  </si>
+  <si>
+    <t>burials having the same gender to be connected</t>
+  </si>
+  <si>
+    <t>burials having the same ritual treatment to be connected</t>
+  </si>
+  <si>
+    <t>burials having the same scale of wealth to be connected</t>
+  </si>
+  <si>
+    <t xml:space="preserve">burials to be connected with a third shared burial </t>
+  </si>
+  <si>
+    <t xml:space="preserve">burials with shorter distance to be connected based on kinship-based relations </t>
+  </si>
+  <si>
+    <t>dyadic relationship/dyadcov.distance</t>
+  </si>
+  <si>
+    <t>Number of ties in the network</t>
+  </si>
+  <si>
+    <t>burials being connected with multiple partners</t>
   </si>
 </sst>
 </file>
@@ -502,7 +511,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -516,128 +525,128 @@
   <sheetData>
     <row r="1" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>6</v>
+        <v>34</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="D3" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="D4" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>14</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="C6" s="1" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="B9" s="1" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
edit captions in the rmd and the ergm table
</commit_message>
<xml_diff>
--- a/analysis/data/raw_data/ergm_term.xlsx
+++ b/analysis/data/raw_data/ergm_term.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/EmilyWang/Desktop/School document/LW-Papers/kwl-burials-2020/analysis/data/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82BD63F9-7601-834D-99FC-DCD15E87A46C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE85E8E5-CEC9-8E4F-9B4F-131565C73E26}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30820" yWindow="2440" windowWidth="20020" windowHeight="16560" xr2:uid="{9B72E976-F785-7749-915A-031B6E0C4CD8}"/>
   </bookViews>
@@ -38,9 +38,6 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Interpretation</t>
-  </si>
-  <si>
     <t>Edges</t>
   </si>
   <si>
@@ -68,12 +65,6 @@
     <t>Density of ties between nodes with the same gender</t>
   </si>
   <si>
-    <t>Network Property</t>
-  </si>
-  <si>
-    <t>Configurations (effect/parameter)</t>
-  </si>
-  <si>
     <t>Transitivity or cohesion</t>
   </si>
   <si>
@@ -141,6 +132,15 @@
   </si>
   <si>
     <t>burials being connected with multiple partners</t>
+  </si>
+  <si>
+    <t>Network Properties</t>
+  </si>
+  <si>
+    <t>Configurations (effects/parameters)</t>
+  </si>
+  <si>
+    <t>Archaeological Interpretation</t>
   </si>
 </sst>
 </file>
@@ -511,7 +511,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -525,128 +525,128 @@
   <sheetData>
     <row r="1" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>11</v>
+        <v>33</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>1</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="C5" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>6</v>
-      </c>
       <c r="D8" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
udpate the table of ERGMs terms
</commit_message>
<xml_diff>
--- a/analysis/data/raw_data/ergm_term.xlsx
+++ b/analysis/data/raw_data/ergm_term.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/EmilyWang/Desktop/School document/LW-Papers/kwl-burials-2020/analysis/data/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE85E8E5-CEC9-8E4F-9B4F-131565C73E26}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88B3170C-F2E1-EA44-AB5E-3BC7ECC21466}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30820" yWindow="2440" windowWidth="20020" windowHeight="16560" xr2:uid="{9B72E976-F785-7749-915A-031B6E0C4CD8}"/>
   </bookViews>
@@ -56,9 +56,6 @@
     <t>Density of ties between nodes with same scale of wealth</t>
   </si>
   <si>
-    <t>Density of ties between nodes with same ritual treatment</t>
-  </si>
-  <si>
     <t>Density of ties between nodes with the same age</t>
   </si>
   <si>
@@ -101,9 +98,6 @@
     <t>physical distance</t>
   </si>
   <si>
-    <t>Distance (in meter) between each pairs of burials</t>
-  </si>
-  <si>
     <t>two burials having relationship</t>
   </si>
   <si>
@@ -141,6 +135,12 @@
   </si>
   <si>
     <t>Archaeological Interpretation</t>
+  </si>
+  <si>
+    <t>Distance (in meter) between each pair of burials</t>
+  </si>
+  <si>
+    <t>Density of ties between nodes with the same ritual treatment</t>
   </si>
 </sst>
 </file>
@@ -511,7 +511,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -525,16 +525,16 @@
   <sheetData>
     <row r="1" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -545,80 +545,80 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>7</v>
+        <v>35</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>17</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -626,27 +626,27 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update the table for ergm term
</commit_message>
<xml_diff>
--- a/analysis/data/raw_data/ergm_term.xlsx
+++ b/analysis/data/raw_data/ergm_term.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/EmilyWang/Desktop/School document/LW-Papers/kwl-burials-2020/analysis/data/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88B3170C-F2E1-EA44-AB5E-3BC7ECC21466}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27C5A5EC-1443-5F45-BA3E-2B332D71D02F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30820" yWindow="2440" windowWidth="20020" windowHeight="16560" xr2:uid="{9B72E976-F785-7749-915A-031B6E0C4CD8}"/>
+    <workbookView xWindow="36820" yWindow="3020" windowWidth="20020" windowHeight="16560" xr2:uid="{9B72E976-F785-7749-915A-031B6E0C4CD8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,107 +33,32 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="35">
   <si>
     <t>Description</t>
   </si>
   <si>
-    <t>Edges</t>
-  </si>
-  <si>
-    <t>Density</t>
-  </si>
-  <si>
     <t xml:space="preserve">Tendency for nodes with shared partners to be tied </t>
   </si>
   <si>
-    <t>Popularity</t>
-  </si>
-  <si>
     <t>Tendency towards centralization in distribution</t>
   </si>
   <si>
-    <t>Density of ties between nodes with same scale of wealth</t>
-  </si>
-  <si>
     <t>Density of ties between nodes with the same age</t>
   </si>
   <si>
     <t>Density of ties between nodes with the same gender</t>
   </si>
   <si>
-    <t>Transitivity or cohesion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Homophily/nodematch.age </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Homophily/nodematch.sex </t>
-  </si>
-  <si>
-    <t>Node covariate of age</t>
-  </si>
-  <si>
-    <t>Node covariate of sex</t>
-  </si>
-  <si>
-    <t>Node covariate of ritual pottery</t>
-  </si>
-  <si>
-    <t>Node covariate of burial value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Homophily/nodematch.value </t>
-  </si>
-  <si>
-    <t>Homophily/nodematch.ritual</t>
-  </si>
-  <si>
     <t>Geometrically weighted edgewise shared partner (gwesp)</t>
   </si>
   <si>
-    <t>geometrically weighted degree distribution (gwdeg)</t>
-  </si>
-  <si>
-    <t>physical distance</t>
-  </si>
-  <si>
-    <t>two burials having relationship</t>
-  </si>
-  <si>
-    <t>burials having the same age to be connected</t>
-  </si>
-  <si>
-    <t>burials having the same gender to be connected</t>
-  </si>
-  <si>
-    <t>burials having the same ritual treatment to be connected</t>
-  </si>
-  <si>
-    <t>burials having the same scale of wealth to be connected</t>
-  </si>
-  <si>
-    <t xml:space="preserve">burials to be connected with a third shared burial </t>
-  </si>
-  <si>
-    <t xml:space="preserve">burials with shorter distance to be connected based on kinship-based relations </t>
-  </si>
-  <si>
-    <t>dyadic relationship/dyadcov.distance</t>
-  </si>
-  <si>
     <t>Number of ties in the network</t>
   </si>
   <si>
     <t>burials being connected with multiple partners</t>
   </si>
   <si>
-    <t>Network Properties</t>
-  </si>
-  <si>
-    <t>Configurations (effects/parameters)</t>
-  </si>
-  <si>
     <t>Archaeological Interpretation</t>
   </si>
   <si>
@@ -141,6 +66,78 @@
   </si>
   <si>
     <t>Density of ties between nodes with the same ritual treatment</t>
+  </si>
+  <si>
+    <t>or cohesion</t>
+  </si>
+  <si>
+    <t>Network variable</t>
+  </si>
+  <si>
+    <t>Physical distance</t>
+  </si>
+  <si>
+    <t>Geometrically weighted degree distribution (gwdegree)</t>
+  </si>
+  <si>
+    <t>Uniform homophily (nodematch)</t>
+  </si>
+  <si>
+    <t>Dyadic covariate (dyadcov)</t>
+  </si>
+  <si>
+    <t>note</t>
+  </si>
+  <si>
+    <t>Configuration (term in ERGM)</t>
+  </si>
+  <si>
+    <t>Edges (edges)</t>
+  </si>
+  <si>
+    <t>Density of ties between nodes with the same scale of wealth</t>
+  </si>
+  <si>
+    <t>constituent element of the network</t>
+  </si>
+  <si>
+    <t>burials in the same age tend to have similar goods</t>
+  </si>
+  <si>
+    <t>burials in the same sex tend to have similar goods</t>
+  </si>
+  <si>
+    <t>burials having ritual practice tend to have similar goods</t>
+  </si>
+  <si>
+    <t xml:space="preserve">burials in the same wealth rank tend to have similar goods </t>
+  </si>
+  <si>
+    <t xml:space="preserve">burials close to each other tend to have simialr goods </t>
+  </si>
+  <si>
+    <t>burials being connected with a third burial</t>
+  </si>
+  <si>
+    <t>Density/inter-relation</t>
+  </si>
+  <si>
+    <t>Age-homophily</t>
+  </si>
+  <si>
+    <t>Sex-homophily</t>
+  </si>
+  <si>
+    <t>Ritual-homophily</t>
+  </si>
+  <si>
+    <t>Wealth-homophily</t>
+  </si>
+  <si>
+    <t>Transitivity/clustering</t>
+  </si>
+  <si>
+    <t>Centralization</t>
   </si>
 </sst>
 </file>
@@ -508,145 +505,152 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25AEFDEF-7A8C-D44E-A75C-8E7C98450230}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="32.83203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="23" style="1" customWidth="1"/>
     <col min="2" max="2" width="32" style="1" customWidth="1"/>
     <col min="3" max="3" width="27.33203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="26" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="10.83203125" style="1"/>
+    <col min="4" max="5" width="26" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="B6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="B7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+    </row>
+    <row r="9" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="51" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="51" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
+      <c r="C9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="51" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
edit the main text in paper rmd
</commit_message>
<xml_diff>
--- a/analysis/data/raw_data/ergm_term.xlsx
+++ b/analysis/data/raw_data/ergm_term.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/EmilyWang/Desktop/School document/LW-Papers/kwl-burials-2020/analysis/data/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27C5A5EC-1443-5F45-BA3E-2B332D71D02F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABFCC180-BF77-1A47-81DB-9AC5D45546EF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36820" yWindow="3020" windowWidth="20020" windowHeight="16560" xr2:uid="{9B72E976-F785-7749-915A-031B6E0C4CD8}"/>
+    <workbookView xWindow="3520" yWindow="880" windowWidth="20020" windowHeight="16560" xr2:uid="{9B72E976-F785-7749-915A-031B6E0C4CD8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -89,9 +89,6 @@
     <t>note</t>
   </si>
   <si>
-    <t>Configuration (term in ERGM)</t>
-  </si>
-  <si>
     <t>Edges (edges)</t>
   </si>
   <si>
@@ -137,7 +134,10 @@
     <t>Transitivity/clustering</t>
   </si>
   <si>
-    <t>Centralization</t>
+    <t>Configuration (ERGM term)</t>
+  </si>
+  <si>
+    <t>Centralization/popularity</t>
   </si>
 </sst>
 </file>
@@ -508,7 +508,7 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -525,7 +525,7 @@
         <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>8</v>
@@ -539,13 +539,13 @@
     </row>
     <row r="2" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>6</v>
@@ -554,13 +554,13 @@
     </row>
     <row r="3" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>3</v>
@@ -568,13 +568,13 @@
     </row>
     <row r="4" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>4</v>
@@ -582,13 +582,13 @@
     </row>
     <row r="5" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>10</v>
@@ -596,27 +596,27 @@
     </row>
     <row r="6" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>1</v>
@@ -647,7 +647,7 @@
         <v>16</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
edits to the text after peer review and revisions
</commit_message>
<xml_diff>
--- a/analysis/data/raw_data/ergm_term.xlsx
+++ b/analysis/data/raw_data/ergm_term.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/EmilyWang/Desktop/School document/LW-Papers/kwl-burials-2020/analysis/data/raw_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bmarwick/Desktop/kwl-burials/analysis/data/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8585C2F0-9646-9C45-9E3A-6E353CC1F322}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDF1FDCA-0F73-9142-9FBD-6C5E39DAE627}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3520" yWindow="460" windowWidth="20020" windowHeight="16560" xr2:uid="{9B72E976-F785-7749-915A-031B6E0C4CD8}"/>
+    <workbookView xWindow="9240" yWindow="620" windowWidth="18160" windowHeight="16560" xr2:uid="{9B72E976-F785-7749-915A-031B6E0C4CD8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,14 +20,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -56,9 +48,6 @@
     <t>Number of ties in the network</t>
   </si>
   <si>
-    <t>burials being connected with multiple partners</t>
-  </si>
-  <si>
     <t>Archaeological Interpretation</t>
   </si>
   <si>
@@ -95,24 +84,6 @@
     <t>Density of ties between nodes with the same scale of wealth</t>
   </si>
   <si>
-    <t>constituent element of the network</t>
-  </si>
-  <si>
-    <t>burials in the same age tend to have similar goods</t>
-  </si>
-  <si>
-    <t>burials in the same sex tend to have similar goods</t>
-  </si>
-  <si>
-    <t>burials having ritual practice tend to have similar goods</t>
-  </si>
-  <si>
-    <t xml:space="preserve">burials in the same wealth rank tend to have similar goods </t>
-  </si>
-  <si>
-    <t>burials being connected with a third burial</t>
-  </si>
-  <si>
     <t>Density/inter-relation</t>
   </si>
   <si>
@@ -137,7 +108,28 @@
     <t>Centralization/popularity</t>
   </si>
   <si>
-    <t xml:space="preserve">burials close to each other tend to have similar goods </t>
+    <t>Constituent element of the network</t>
+  </si>
+  <si>
+    <t>Burials in the same age tend to have similar goods</t>
+  </si>
+  <si>
+    <t>Burials of the same sex tend to have similar goods</t>
+  </si>
+  <si>
+    <t>Burials having ritual practice tend to have similar goods</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Burials in the same wealth rank tend to have similar goods </t>
+  </si>
+  <si>
+    <t>Two burials being connected with a third burial</t>
+  </si>
+  <si>
+    <t>Burials being connected with multiple partners</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Burials physically close to each other tend to have similar goods </t>
   </si>
 </sst>
 </file>
@@ -508,7 +500,7 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -522,30 +514,30 @@
   <sheetData>
     <row r="1" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>6</v>
@@ -554,13 +546,13 @@
     </row>
     <row r="3" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>3</v>
@@ -568,13 +560,13 @@
     </row>
     <row r="4" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>4</v>
@@ -582,75 +574,75 @@
     </row>
     <row r="5" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>7</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>34</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>